<commit_message>
Update EffortLog + Weekly Report
</commit_message>
<xml_diff>
--- a/1.DELIVERABLE/1.10 EFFORT_LOG/Week25/BSS_EffortLog_XuanThaiHien_Week25.xlsx
+++ b/1.DELIVERABLE/1.10 EFFORT_LOG/Week25/BSS_EffortLog_XuanThaiHien_Week25.xlsx
@@ -42,7 +42,7 @@
     <t>Actual Time</t>
   </si>
   <si>
-    <t>WEEK: 20</t>
+    <t>WEEK: 25</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -495,7 +495,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>